<commit_message>
Final Version But I'm not sure...
</commit_message>
<xml_diff>
--- a/generation/download.xlsx
+++ b/generation/download.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -140,7 +135,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -580,7 +575,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -593,8 +588,8 @@
   </sheetPr>
   <dimension ref="A1:J415"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,7 +799,7 @@
     </row>
     <row r="16" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
-        <v>43344</v>
+        <v>43507</v>
       </c>
       <c r="B16" s="7">
         <v>8</v>
@@ -836,7 +831,7 @@
     </row>
     <row r="17" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
-        <v>43345</v>
+        <v>43508</v>
       </c>
       <c r="B17" s="7">
         <v>7</v>
@@ -868,7 +863,7 @@
     </row>
     <row r="18" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
-        <v>43346</v>
+        <v>43509</v>
       </c>
       <c r="B18" s="7">
         <v>8</v>
@@ -899,7 +894,9 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
+      <c r="A19" s="6">
+        <v>43510</v>
+      </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -911,7 +908,9 @@
       <c r="J19" s="4"/>
     </row>
     <row r="20" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
+      <c r="A20" s="6">
+        <v>43511</v>
+      </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -923,7 +922,9 @@
       <c r="J20" s="4"/>
     </row>
     <row r="21" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
+      <c r="A21" s="6">
+        <v>43512</v>
+      </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -935,7 +936,9 @@
       <c r="J21" s="4"/>
     </row>
     <row r="22" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
+      <c r="A22" s="6">
+        <v>43513</v>
+      </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -947,7 +950,9 @@
       <c r="J22" s="4"/>
     </row>
     <row r="23" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
+      <c r="A23" s="6">
+        <v>43514</v>
+      </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -959,7 +964,9 @@
       <c r="J23" s="4"/>
     </row>
     <row r="24" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
+      <c r="A24" s="6">
+        <v>43515</v>
+      </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -971,7 +978,9 @@
       <c r="J24" s="4"/>
     </row>
     <row r="25" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
+      <c r="A25" s="6">
+        <v>43516</v>
+      </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -983,7 +992,9 @@
       <c r="J25" s="4"/>
     </row>
     <row r="26" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
+      <c r="A26" s="6">
+        <v>43517</v>
+      </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -995,7 +1006,9 @@
       <c r="J26" s="4"/>
     </row>
     <row r="27" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
+      <c r="A27" s="6">
+        <v>43518</v>
+      </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -1007,7 +1020,9 @@
       <c r="J27" s="4"/>
     </row>
     <row r="28" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
+      <c r="A28" s="6">
+        <v>43519</v>
+      </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -1019,7 +1034,9 @@
       <c r="J28" s="4"/>
     </row>
     <row r="29" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
+      <c r="A29" s="6">
+        <v>43520</v>
+      </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -1031,7 +1048,9 @@
       <c r="J29" s="4"/>
     </row>
     <row r="30" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
+      <c r="A30" s="6">
+        <v>43521</v>
+      </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -1043,7 +1062,9 @@
       <c r="J30" s="4"/>
     </row>
     <row r="31" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
+      <c r="A31" s="6">
+        <v>43522</v>
+      </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
@@ -1055,7 +1076,9 @@
       <c r="J31" s="4"/>
     </row>
     <row r="32" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
+      <c r="A32" s="6">
+        <v>43523</v>
+      </c>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
@@ -1067,7 +1090,9 @@
       <c r="J32" s="4"/>
     </row>
     <row r="33" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
+      <c r="A33" s="6">
+        <v>43524</v>
+      </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -1079,7 +1104,9 @@
       <c r="J33" s="4"/>
     </row>
     <row r="34" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="4"/>
+      <c r="A34" s="6">
+        <v>43525</v>
+      </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
@@ -1091,7 +1118,9 @@
       <c r="J34" s="4"/>
     </row>
     <row r="35" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="4"/>
+      <c r="A35" s="6">
+        <v>43526</v>
+      </c>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>

</xml_diff>